<commit_message>
Switch all DK to ENG
</commit_message>
<xml_diff>
--- a/2021-0313846_slurry_separation/manuscript work/EF_calcs/inputs/inputs.xlsx
+++ b/2021-0313846_slurry_separation/manuscript work/EF_calcs/inputs/inputs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Field app scenarios" sheetId="1" state="visible" r:id="rId2"/>
@@ -197,13 +197,13 @@
     <t xml:space="preserve">man.ph</t>
   </si>
   <si>
-    <t xml:space="preserve">Svinegylle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kvæggylle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Afgasset biomasse</t>
+    <t xml:space="preserve">Pig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cattle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digestate</t>
   </si>
   <si>
     <t xml:space="preserve">app.timing</t>
@@ -218,19 +218,19 @@
     <t xml:space="preserve">rain.rate</t>
   </si>
   <si>
-    <t xml:space="preserve">Marts</t>
+    <t xml:space="preserve">March</t>
   </si>
   <si>
     <t xml:space="preserve">April</t>
   </si>
   <si>
-    <t xml:space="preserve">Maj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sommer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Efterår</t>
+    <t xml:space="preserve">May</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Summer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autumn</t>
   </si>
   <si>
     <t xml:space="preserve">sep.eff.TAN</t>
@@ -340,7 +340,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -379,6 +379,10 @@
     </xf>
     <xf numFmtId="170" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -460,7 +464,7 @@
   </sheetPr>
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -506,7 +510,8 @@
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="b">
+      <c r="B2" s="4" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C2" s="3"/>
@@ -525,7 +530,8 @@
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="4" t="b">
+      <c r="B3" s="4" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C3" s="3"/>
@@ -544,7 +550,8 @@
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="4" t="b">
+      <c r="B4" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C4" s="3" t="n">
@@ -570,7 +577,8 @@
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4" t="b">
+      <c r="B5" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C5" s="3" t="n">
@@ -596,7 +604,8 @@
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="4" t="b">
+      <c r="B6" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C6" s="3" t="n">
@@ -622,7 +631,8 @@
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="4" t="b">
+      <c r="B7" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C7" s="3" t="n">
@@ -648,7 +658,8 @@
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4" t="b">
+      <c r="B8" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C8" s="3" t="n">
@@ -674,7 +685,8 @@
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="4" t="b">
+      <c r="B9" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C9" s="3" t="n">
@@ -700,7 +712,8 @@
       <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="4" t="b">
+      <c r="B10" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C10" s="3" t="n">
@@ -726,7 +739,8 @@
       <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="4" t="b">
+      <c r="B11" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C11" s="3" t="n">
@@ -752,7 +766,8 @@
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="4" t="b">
+      <c r="B12" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C12" s="3" t="n">
@@ -782,7 +797,8 @@
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="4" t="b">
+      <c r="B13" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C13" s="3" t="n">
@@ -812,7 +828,8 @@
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="4" t="b">
+      <c r="B14" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C14" s="3" t="n">
@@ -842,7 +859,8 @@
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="4" t="b">
+      <c r="B15" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C15" s="3" t="n">
@@ -872,7 +890,8 @@
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="4" t="b">
+      <c r="B16" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C16" s="3" t="n">
@@ -902,7 +921,8 @@
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="4" t="b">
+      <c r="B17" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C17" s="3" t="n">
@@ -932,7 +952,8 @@
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="4" t="b">
+      <c r="B18" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C18" s="3" t="n">
@@ -962,7 +983,8 @@
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="4" t="b">
+      <c r="B19" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C19" s="3" t="n">
@@ -1039,10 +1061,10 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.12890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="16.86"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1016" min="2" style="3" width="10.13"/>
@@ -1111,10 +1133,10 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.13671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.12890625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="12.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="8"/>
@@ -1229,7 +1251,7 @@
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.13671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.12890625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="10.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="10.42"/>
@@ -1298,10 +1320,10 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.13671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.12890625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="10.57"/>
@@ -1404,25 +1426,25 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="10" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="10" t="n">
         <v>168</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="10" t="n">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix SF application issue.
Changes overall EF so they now look the same as in the meom.
</commit_message>
<xml_diff>
--- a/2021-0313846_slurry_separation/manuscript work/EF_calcs/inputs/inputs.xlsx
+++ b/2021-0313846_slurry_separation/manuscript work/EF_calcs/inputs/inputs.xlsx
@@ -22,6 +22,30 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>SDH</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Sans"/>
+            <family val="0"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">For raw slurry and for liquid fraction.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -143,7 +167,7 @@
     <t xml:space="preserve">dpH</t>
   </si>
   <si>
-    <t xml:space="preserve">app.mthd</t>
+    <t xml:space="preserve">app.mthd.rl</t>
   </si>
   <si>
     <t xml:space="preserve">app.mthd.sf</t>
@@ -465,7 +489,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I12" activeCellId="0" sqref="I12:I19"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -474,7 +498,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="11.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="11.18"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="7" style="1" width="10.08"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="7" style="1" width="10.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1050,6 +1074,7 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1061,7 +1086,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="I12:I19 A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.12890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1133,7 +1158,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="I12:I19 A7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.12890625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1248,7 +1273,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="1" sqref="I12:I19 B5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.12890625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1320,7 +1345,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="I12:I19 A5"/>
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.12890625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1427,7 +1452,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="1" sqref="I12:I19 C8"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.08203125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>